<commit_message>
Added ability to read strNameLen from info.csv
</commit_message>
<xml_diff>
--- a/infoKeyChain.xlsx
+++ b/infoKeyChain.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hans-Christian\PycharmProjects\AddTextToDXF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA92E76-3B75-4C7B-8031-C61CC0D259B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2B8C5B-98D8-4BDB-9148-318DD3CA2680}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1210" yWindow="2210" windowWidth="14400" windowHeight="7450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>finalFileName</t>
   </si>
@@ -76,22 +76,34 @@
     <t>textHeight</t>
   </si>
   <si>
+    <t>strNameLen</t>
+  </si>
+  <si>
     <t>testPlate.dxf</t>
   </si>
   <si>
-    <t>NTNU_Plate_Template_v1.dxf</t>
-  </si>
-  <si>
-    <t>logo_ntnu_manulab.png</t>
-  </si>
-  <si>
-    <t>Julius Andreas Gimli Arn MacGyver Chewbacka Highlander Elessar-Jankov</t>
+    <t>NTNU_KeyChain_Template_v2.dxf</t>
+  </si>
+  <si>
+    <t>ntnu_logo_svart.png</t>
+  </si>
+  <si>
+    <t>18.7732</t>
+  </si>
+  <si>
+    <t>JAGAMcGCHE-J</t>
   </si>
   <si>
     <t>NTNU-DIN</t>
   </si>
   <si>
+    <t>1.5050</t>
+  </si>
+  <si>
     <t>29.5</t>
+  </si>
+  <si>
+    <t>12.5</t>
   </si>
   <si>
     <t>2.5</t>
@@ -936,15 +948,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -999,22 +1011,25 @@
       <c r="R1" t="s">
         <v>17</v>
       </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>60</v>
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
       </c>
       <c r="F2">
         <v>260</v>
@@ -1026,22 +1041,22 @@
         <v>22</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="L2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2">
-        <v>50</v>
+        <v>24</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="N2">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="O2">
         <v>0</v>
@@ -1053,7 +1068,10 @@
         <v>25</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
+      </c>
+      <c r="S2">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>